<commit_message>
adding newly added test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="616" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,17 @@
     <sheet name="ResetPassword" sheetId="7" r:id="rId4"/>
     <sheet name="LoginPageDataProvider" sheetId="8" r:id="rId5"/>
     <sheet name="AddUser" sheetId="9" r:id="rId6"/>
+    <sheet name="AddUserDetails" sheetId="10" r:id="rId7"/>
+    <sheet name="EditUserPage" sheetId="11" r:id="rId8"/>
+    <sheet name="RolesPage" sheetId="12" r:id="rId9"/>
+    <sheet name="AddRolesPage" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Title</t>
   </si>
@@ -78,23 +82,116 @@
     <t>userName</t>
   </si>
   <si>
-    <t>Anu</t>
-  </si>
-  <si>
-    <t>anumeenu2610@gmail.com</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
     <t>anumeenu</t>
+  </si>
+  <si>
+    <t>randomUname</t>
+  </si>
+  <si>
+    <t>efgh</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>No matching records found</t>
+  </si>
+  <si>
+    <t>alpharittu</t>
+  </si>
+  <si>
+    <t>alpha114@gmail.com</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>Add user - QAlegend</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>ritty</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>Edit user - QAlegend</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>benin</t>
+  </si>
+  <si>
+    <t>deleteUser</t>
+  </si>
+  <si>
+    <t>abianu</t>
+  </si>
+  <si>
+    <t>tilte</t>
+  </si>
+  <si>
+    <t>Roles - QAlegend</t>
+  </si>
+  <si>
+    <t>minnu</t>
+  </si>
+  <si>
+    <t>minnu123@gmail.com</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>This field is required.</t>
+  </si>
+  <si>
+    <t>newlyaddeduser</t>
+  </si>
+  <si>
+    <t>newuserpass</t>
+  </si>
+  <si>
+    <t>Add Role - QAlegend</t>
+  </si>
+  <si>
+    <t>viewUser</t>
+  </si>
+  <si>
+    <t>abianu123@gmail.com</t>
+  </si>
+  <si>
+    <t>rolename</t>
+  </si>
+  <si>
+    <t>edit rolespage title</t>
+  </si>
+  <si>
+    <t>Edit Role - QAlegend</t>
+  </si>
+  <si>
+    <t>QA Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +222,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -161,6 +271,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -464,19 +589,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" customWidth="1"/>
     <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,24 +617,67 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>123456</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -541,25 +712,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -640,16 +831,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" customWidth="1"/>
     <col min="2" max="2" width="26.08984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -663,33 +857,33 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>123456</v>
+      <c r="D2" t="s">
+        <v>27</v>
       </c>
       <c r="E2">
         <v>123456</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
+      <c r="F2">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -697,5 +891,165 @@
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.08984375" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new changes adding to git
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="616" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="767" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="EditUserPage" sheetId="11" r:id="rId8"/>
     <sheet name="RolesPage" sheetId="12" r:id="rId9"/>
     <sheet name="AddRolesPage" sheetId="13" r:id="rId10"/>
+    <sheet name="SalesPage" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>Title</t>
   </si>
@@ -185,6 +186,57 @@
   </si>
   <si>
     <t>QA Tester</t>
+  </si>
+  <si>
+    <t>rolename2</t>
+  </si>
+  <si>
+    <t>Qa Testing 2</t>
+  </si>
+  <si>
+    <t>rolesname3</t>
+  </si>
+  <si>
+    <t>QA testing 4</t>
+  </si>
+  <si>
+    <t>deleterole</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Sales Commission Agents - QAlegend</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>anu</t>
+  </si>
+  <si>
+    <t>meenu</t>
+  </si>
+  <si>
+    <t>anu123@gmail.com</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>editlastname</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>deletesales</t>
   </si>
 </sst>
 </file>
@@ -257,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -287,6 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -652,32 +705,139 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
+      <c r="C2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2">
+        <v>1234567890</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>